<commit_message>
tune prefer local district services
</commit_message>
<xml_diff>
--- a/METM_Analysis.xlsx
+++ b/METM_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wip\cs-mod-dev\MoreEffectiveTransfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39347F82-9368-41F6-9805-ACD274F90C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2006375-10DC-4D88-8BD5-0A918DA233D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Additional mods to gather statistics:</t>
   </si>
@@ -109,12 +109,6 @@
     <t>- VANILLA TRANSFER MANAGER: NUM INVOCATIONS: 213164, TOTAL MS: 83101, AVG TIME/INVOCATION: 0.3898454ms</t>
   </si>
   <si>
-    <t>Run #1: METM - 1 year NONE ENABLED (19.09.20199)</t>
-  </si>
-  <si>
-    <t>Run #1: METM - 1 year ONLY WH1st ENABLED (19.09.20199)</t>
-  </si>
-  <si>
     <t>Run #1: METM - 8mths ALL ENABLED (01.05.20199)</t>
   </si>
   <si>
@@ -122,6 +116,18 @@
   </si>
   <si>
     <t>-     NEW TRANSFER MANAGER: NUM INVOCATIONS: 130652, TOTAL MS: 54625, AVG TIME/INVOCATION: 0.4180954ms</t>
+  </si>
+  <si>
+    <t>Run #1: METM - 9mths NONE ENABLED (20.06.20199)</t>
+  </si>
+  <si>
+    <t>~350,000</t>
+  </si>
+  <si>
+    <t>-     NEW TRANSFER MANAGER: NUM INVOCATIONS: 160056, TOTAL MS: 64400, AVG TIME/INVOCATION: 0.4023592ms</t>
+  </si>
+  <si>
+    <t>Run #2: VANILLA - 1 year (19.09.2199)</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +719,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="11">
         <v>319465</v>
@@ -743,7 +749,7 @@
         <v>0.86</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L12" s="9">
         <v>13000</v>
@@ -752,17 +758,53 @@
         <v>0.41809540000000001</v>
       </c>
       <c r="N12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="B13" s="11">
+        <v>308000</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="E13">
+        <v>6227</v>
+      </c>
+      <c r="F13" s="9">
+        <v>11737</v>
+      </c>
+      <c r="G13" s="9">
+        <v>3100</v>
+      </c>
+      <c r="H13">
+        <v>7690</v>
+      </c>
+      <c r="I13">
+        <v>7000</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.89</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13">
+        <v>12200</v>
+      </c>
+      <c r="M13">
+        <v>0.40235919999999997</v>
+      </c>
+      <c r="N13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tune local district formula
</commit_message>
<xml_diff>
--- a/METM_Analysis.xlsx
+++ b/METM_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wip\cs-mod-dev\MoreEffectiveTransfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F66CDCF-649D-4ABE-A776-65489D1DA4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A40F68-3226-4DAA-9690-E362AC5E0A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Additional mods to gather statistics:</t>
   </si>
@@ -124,10 +124,13 @@
     <t>-     NEW TRANSFER MANAGER: NUM INVOCATIONS: 160056, TOTAL MS: 64400, AVG TIME/INVOCATION: 0.4023592ms</t>
   </si>
   <si>
-    <t>Run #2: VANILLA - 1 year (19.09.2199)</t>
-  </si>
-  <si>
     <t>"Cim City" (Vanilla.crp) by ThisHero</t>
+  </si>
+  <si>
+    <t>Run #2: VANILLA - 16mths (01.04.2199)</t>
+  </si>
+  <si>
+    <t>- VANILLA TRANSFER MANAGER: NUM INVOCATIONS: 113104, TOTAL MS: 43310, AVG TIME/INVOCATION: 0.3829219ms</t>
   </si>
 </sst>
 </file>
@@ -246,7 +249,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -268,6 +271,10 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -555,7 +562,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,8 +576,8 @@
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
     <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -579,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" t="s">
@@ -824,9 +831,48 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>30</v>
+    <row r="14" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="17">
+        <v>320000</v>
+      </c>
+      <c r="C14" s="21">
+        <v>0.04</v>
+      </c>
+      <c r="D14" s="22">
+        <v>-77000</v>
+      </c>
+      <c r="E14" s="16">
+        <v>6076</v>
+      </c>
+      <c r="F14" s="16">
+        <v>9963</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1880</v>
+      </c>
+      <c r="H14" s="16">
+        <v>6179</v>
+      </c>
+      <c r="I14" s="16">
+        <v>5400</v>
+      </c>
+      <c r="J14" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="16">
+        <v>12300</v>
+      </c>
+      <c r="M14" s="16">
+        <v>0.38292189999999998</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REJECT_LOW_PRIORITY, move some code, inlining options
</commit_message>
<xml_diff>
--- a/METM_Analysis.xlsx
+++ b/METM_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wip\cs-mod-dev\MoreEffectiveTransfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A40F68-3226-4DAA-9690-E362AC5E0A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8AE408-A283-4E0D-BA90-71F2B78513E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Additional mods to gather statistics:</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>- VANILLA TRANSFER MANAGER: NUM INVOCATIONS: 113104, TOTAL MS: 43310, AVG TIME/INVOCATION: 0.3829219ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run #2: METM - ALL OPTIONS ON continued from 01.04. to </t>
   </si>
 </sst>
 </file>
@@ -559,15 +562,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -875,6 +878,11 @@
         <v>32</v>
       </c>
     </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
improve logging, add init checks
</commit_message>
<xml_diff>
--- a/METM_Analysis.xlsx
+++ b/METM_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wip\cs-mod-dev\MoreEffectiveTransfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8AE408-A283-4E0D-BA90-71F2B78513E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D58A5F5-ECA2-4CA0-AE9B-5A6624F1E5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Additional mods to gather statistics:</t>
   </si>
@@ -133,7 +133,22 @@
     <t>- VANILLA TRANSFER MANAGER: NUM INVOCATIONS: 113104, TOTAL MS: 43310, AVG TIME/INVOCATION: 0.3829219ms</t>
   </si>
   <si>
-    <t xml:space="preserve">Run #2: METM - ALL OPTIONS ON continued from 01.04. to </t>
+    <t>Run #3: VANILLA - 1 month (20.10.2199)</t>
+  </si>
+  <si>
+    <t>Run #3: METM (MONO AOT) - 1 month (20.10.2199)</t>
+  </si>
+  <si>
+    <t>- VANILLA TRANSFER MANAGER: NUM INVOCATIONS: 17724, TOTAL MS: 7699, AVG TIME/INVOCATION: 0.4343828ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                then METM 1mo (20.11.2199)</t>
+  </si>
+  <si>
+    <t>-     NEW TRANSFER MANAGER: NUM INVOCATIONS: 18136, TOTAL MS: 7374, AVG TIME/INVOCATION: 0.4065946ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                then Vanilla 1mo (20.11.2199)</t>
   </si>
 </sst>
 </file>
@@ -252,7 +267,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -274,10 +289,12 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -562,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,53 +851,80 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="22">
         <v>320000</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="23">
         <v>0.04</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="24">
         <v>-77000</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="21">
         <v>6076</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="21">
         <v>9963</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="21">
         <v>1880</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="21">
         <v>6179</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="21">
         <v>5400</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="25">
         <v>0.9</v>
       </c>
-      <c r="K14" s="24" t="s">
+      <c r="K14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="21">
         <v>12300</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="21">
         <v>0.38292189999999998</v>
       </c>
-      <c r="N14" s="16" t="s">
+      <c r="N14" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.43438280000000001</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.40659459999999997</v>
+      </c>
+      <c r="N16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>